<commit_message>
Codes according to php
</commit_message>
<xml_diff>
--- a/Backend/uploads/Updated List.xlsx
+++ b/Backend/uploads/Updated List.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prince\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC8FB5-B3C7-45CD-9614-F414AB14B2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832744CC-2DB6-404E-9163-41D556C68467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="99acres (1)" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'99acres (1)'!$A$1:$AC$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -3236,14 +3239,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="10" max="11" width="24" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
@@ -10537,9 +10541,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AC1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" xr:uid="{3EBB1ED8-D490-48B6-B0EB-7B8E5C71380D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>